<commit_message>
force sensor calcs for MSP430 ADC to detemrine optimal V supply and pulldown resistor. Some MSP code
</commit_message>
<xml_diff>
--- a/Peripheral Code/Force Sensor/Calibration Data.xlsx
+++ b/Peripheral Code/Force Sensor/Calibration Data.xlsx
@@ -5,15 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JasonsRazer\Dropbox\NOTES\MECH 423 - Mechatronic Product Design\PROJECT\MECH423 Project GIT REPO\CyclingDAQ\Peripheral Code\Force Sensor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JasonsRazer\Dropbox\Notes\MECH 423 - Mechatronic Product Design\PROJECT\MECH423 Project GIT REPO\CyclingDAQ\Peripheral Code\Force Sensor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F546E25-0027-483D-83C3-1A28F3753191}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DB4A2BA-BC9E-4BE0-A8C6-FC5265231D96}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{55C83500-F648-47C6-B0AB-D5CA633E4192}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{55C83500-F648-47C6-B0AB-D5CA633E4192}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Calibration" sheetId="1" r:id="rId1"/>
+    <sheet name="Arduino" sheetId="2" r:id="rId2"/>
+    <sheet name="MSP430" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,8 +32,44 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={E9FA19CC-2026-4B7F-B8FC-10CDDFDB7253}</author>
+    <author>tc={6F6BD617-27CB-40F8-A815-561C9B6C09C6}</author>
+    <author>tc={7042F8DC-0326-4603-8611-8624BE808993}</author>
+  </authors>
+  <commentList>
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{E9FA19CC-2026-4B7F-B8FC-10CDDFDB7253}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Measured Vcc on MSP430 was 3.6V</t>
+      </text>
+    </comment>
+    <comment ref="J4" authorId="1" shapeId="0" xr:uid="{6F6BD617-27CB-40F8-A815-561C9B6C09C6}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    will go with this setup</t>
+      </text>
+    </comment>
+    <comment ref="A8" authorId="2" shapeId="0" xr:uid="{7042F8DC-0326-4603-8611-8624BE808993}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Measured Vcc on MSP430 was 3.6V</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="23">
   <si>
     <t>Resistance [kOhm]</t>
   </si>
@@ -74,6 +112,33 @@
   <si>
     <t>Found that 40-50kOhm gives largest dV in 0-5V Vo range Arduino ADC can measure</t>
   </si>
+  <si>
+    <t>Vr-</t>
+  </si>
+  <si>
+    <t>Vr+</t>
+  </si>
+  <si>
+    <t>AVSS</t>
+  </si>
+  <si>
+    <t>AVCC</t>
+  </si>
+  <si>
+    <t>(measured)</t>
+  </si>
+  <si>
+    <t>REF</t>
+  </si>
+  <si>
+    <t>deltaADC</t>
+  </si>
+  <si>
+    <t>Vr- = AVSS // Vr+ = AVCC</t>
+  </si>
+  <si>
+    <t>Vr- = AVSS // Vr+ = REF</t>
+  </si>
 </sst>
 </file>
 
@@ -82,7 +147,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,13 +155,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -111,7 +188,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -125,13 +202,86 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -224,7 +374,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$2</c:f>
+              <c:f>Calibration!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -311,7 +461,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$16</c:f>
+              <c:f>Calibration!$A$3:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -362,7 +512,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$16</c:f>
+              <c:f>Calibration!$B$3:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -1200,6 +1350,122 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>579120</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="https://lh3.googleusercontent.com/7D2E5iSnr1sRyKF6z9CWzpAKgVAJ6fK7BmQShe83u4jLys_sqbBm9iMgmhtGAzxvwQyR-qrgZe-DAz2SY04FZQShoEoeye6nDMhAtPBYw_kSK8sUh8bXUYV4Qm2hPUGe5XGsSJ3a">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0F8DE2E-5090-4AFA-B37B-8F9F7FD589B7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3688080" y="3924300"/>
+          <a:ext cx="5737860" cy="1905000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>586740</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>85304</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>175260</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>24443</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9FA8A3E6-4968-44AD-89E7-05619C9E56C5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3695700" y="1914104"/>
+          <a:ext cx="6606540" cy="2316579"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="jason leblanc" id="{6A9EE71C-D833-42E3-A34D-60E23BE90043}" userId="33f0c2d83078e6ea" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1497,12 +1763,26 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A4" dT="2019-11-30T07:42:23.97" personId="{6A9EE71C-D833-42E3-A34D-60E23BE90043}" id="{E9FA19CC-2026-4B7F-B8FC-10CDDFDB7253}">
+    <text>Measured Vcc on MSP430 was 3.6V</text>
+  </threadedComment>
+  <threadedComment ref="J4" dT="2019-11-30T07:49:35.20" personId="{6A9EE71C-D833-42E3-A34D-60E23BE90043}" id="{6F6BD617-27CB-40F8-A815-561C9B6C09C6}">
+    <text>will go with this setup</text>
+  </threadedComment>
+  <threadedComment ref="A8" dT="2019-11-30T07:42:23.97" personId="{6A9EE71C-D833-42E3-A34D-60E23BE90043}" id="{7042F8DC-0326-4603-8611-8624BE808993}">
+    <text>Measured Vcc on MSP430 was 3.6V</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77B49977-9587-4C45-82F9-1A3FA6065B77}">
-  <dimension ref="A1:T16"/>
+  <dimension ref="A1:T20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1512,10 +1792,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="5"/>
+      <c r="B1" s="6"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -1524,33 +1804,15 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
@@ -1559,38 +1821,15 @@
       <c r="B3" s="1">
         <v>230</v>
       </c>
-      <c r="L3" s="1">
-        <v>5</v>
-      </c>
-      <c r="M3" s="1">
-        <v>1</v>
-      </c>
-      <c r="N3" s="1">
-        <v>20</v>
-      </c>
-      <c r="O3" s="1">
-        <v>47</v>
-      </c>
-      <c r="P3" s="3">
-        <f>(O3/(((N3^-0.654)*119.78)+(O3)))*L3</f>
-        <v>3.6784632265748951</v>
-      </c>
-      <c r="Q3" s="3">
-        <f>(O3/(((M3^-0.654)*119.78)+(O3)))*L3</f>
-        <v>1.4090418515409522</v>
-      </c>
-      <c r="R3" s="2">
-        <f>P3-Q3</f>
-        <v>2.2694213750339429</v>
-      </c>
-      <c r="S3" s="4">
-        <f>1023*(Q3/L3)</f>
-        <v>288.28996282527885</v>
-      </c>
-      <c r="T3" s="4">
-        <f>1023*(P3/L3)</f>
-        <v>752.61357615722352</v>
-      </c>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
@@ -1599,38 +1838,15 @@
       <c r="B4" s="1">
         <v>100</v>
       </c>
-      <c r="L4" s="1">
-        <v>3.3</v>
-      </c>
-      <c r="M4" s="1">
-        <v>1</v>
-      </c>
-      <c r="N4" s="1">
-        <v>20</v>
-      </c>
-      <c r="O4" s="1">
-        <v>47</v>
-      </c>
-      <c r="P4" s="3">
-        <f>(O4/(((N4^-0.654)*119.78)+(O4)))*L4</f>
-        <v>2.4277857295394307</v>
-      </c>
-      <c r="Q4" s="3">
-        <f>(O4/(((M4^-0.654)*119.78)+(O4)))*L4</f>
-        <v>0.92996762201702843</v>
-      </c>
-      <c r="R4" s="2">
-        <f>P4-Q4</f>
-        <v>1.4978181075224022</v>
-      </c>
-      <c r="S4" s="4">
-        <f>1023*(Q4/L4)</f>
-        <v>288.28996282527885</v>
-      </c>
-      <c r="T4" s="4">
-        <f t="shared" ref="T4" si="0">1023*(P4/L4)</f>
-        <v>752.61357615722352</v>
-      </c>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
@@ -1639,6 +1855,11 @@
       <c r="B5" s="1">
         <v>70</v>
       </c>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
@@ -1647,6 +1868,11 @@
       <c r="B6" s="1">
         <v>60</v>
       </c>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -1655,13 +1881,11 @@
       <c r="B7" s="1">
         <v>45</v>
       </c>
-      <c r="L7" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
@@ -1670,11 +1894,11 @@
       <c r="B8" s="1">
         <v>40</v>
       </c>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -1683,6 +1907,11 @@
       <c r="B9" s="1">
         <v>35</v>
       </c>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
@@ -1691,13 +1920,11 @@
       <c r="B10" s="1">
         <v>30</v>
       </c>
-      <c r="L10" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
@@ -1706,11 +1933,11 @@
       <c r="B11" s="1">
         <v>26</v>
       </c>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
@@ -1719,6 +1946,11 @@
       <c r="B12" s="1">
         <v>24</v>
       </c>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
@@ -1752,13 +1984,553 @@
         <v>16</v>
       </c>
     </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B20"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2558F1EF-C414-4FBB-BEC4-AF3CE27A78F8}">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I10" sqref="A1:I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="5">
+        <v>5</v>
+      </c>
+      <c r="B2" s="5">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5">
+        <v>20</v>
+      </c>
+      <c r="D2" s="5">
+        <v>47</v>
+      </c>
+      <c r="E2" s="3">
+        <f>(D2/(((C2^-0.654)*119.78)+(D2)))*A2</f>
+        <v>3.6784632265748951</v>
+      </c>
+      <c r="F2" s="3">
+        <f>(D2/(((B2^-0.654)*119.78)+(D2)))*A2</f>
+        <v>1.4090418515409522</v>
+      </c>
+      <c r="G2" s="2">
+        <f>E2-F2</f>
+        <v>2.2694213750339429</v>
+      </c>
+      <c r="H2" s="4">
+        <f>1023*(F2/A2)</f>
+        <v>288.28996282527885</v>
+      </c>
+      <c r="I2" s="4">
+        <f>1023*(E2/A2)</f>
+        <v>752.61357615722352</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
+        <v>3.3</v>
+      </c>
+      <c r="B3" s="5">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5">
+        <v>20</v>
+      </c>
+      <c r="D3" s="5">
+        <v>47</v>
+      </c>
+      <c r="E3" s="3">
+        <f>(D3/(((C3^-0.654)*119.78)+(D3)))*A3</f>
+        <v>2.4277857295394307</v>
+      </c>
+      <c r="F3" s="3">
+        <f>(D3/(((B3^-0.654)*119.78)+(D3)))*A3</f>
+        <v>0.92996762201702843</v>
+      </c>
+      <c r="G3" s="2">
+        <f>E3-F3</f>
+        <v>1.4978181075224022</v>
+      </c>
+      <c r="H3" s="4">
+        <f>1023*(F3/A3)</f>
+        <v>288.28996282527885</v>
+      </c>
+      <c r="I3" s="4">
+        <f t="shared" ref="I3" si="0">1023*(E3/A3)</f>
+        <v>752.61357615722352</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A6:E7"/>
+    <mergeCell ref="A9:E10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F15F4A7-B3B1-46FF-8C39-09F79D339A4A}">
+  <dimension ref="A1:K23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="3" width="8.88671875" style="9"/>
+    <col min="4" max="4" width="8.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" style="9"/>
+    <col min="11" max="11" width="25.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="9">
+        <v>5</v>
+      </c>
+      <c r="B2" s="9">
+        <v>1</v>
+      </c>
+      <c r="C2" s="9">
+        <v>20</v>
+      </c>
+      <c r="D2" s="9">
+        <v>15</v>
+      </c>
+      <c r="E2" s="10">
+        <f>(D2/(((C2^-0.654)*119.78)+(D2)))*A2</f>
+        <v>2.3521756195978254</v>
+      </c>
+      <c r="F2" s="10">
+        <f>(D2/(((B2^-0.654)*119.78)+(D2)))*A2</f>
+        <v>0.55646238314289953</v>
+      </c>
+      <c r="G2" s="10">
+        <f>E2-F2</f>
+        <v>1.795713236454926</v>
+      </c>
+      <c r="H2" s="11">
+        <f>1023*((F2-$C$11)/($C$13-$C$11))</f>
+        <v>227.7044071820745</v>
+      </c>
+      <c r="I2" s="11">
+        <f>1023*((E2-$C$11)/($C$13-$C$11))</f>
+        <v>962.51026353943018</v>
+      </c>
+      <c r="J2" s="11">
+        <f>I2-H2</f>
+        <v>734.80585635735565</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="9">
+        <v>3.3</v>
+      </c>
+      <c r="B3" s="9">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9">
+        <v>20</v>
+      </c>
+      <c r="D3" s="9">
+        <v>47</v>
+      </c>
+      <c r="E3" s="10">
+        <f>(D3/(((C3^-0.654)*119.78)+(D3)))*A3</f>
+        <v>2.4277857295394307</v>
+      </c>
+      <c r="F3" s="10">
+        <f>(D3/(((B3^-0.654)*119.78)+(D3)))*A3</f>
+        <v>0.92996762201702843</v>
+      </c>
+      <c r="G3" s="10">
+        <f>E3-F3</f>
+        <v>1.4978181075224022</v>
+      </c>
+      <c r="H3" s="11">
+        <f>1023*((F3-$C$11)/($C$13-$C$11))</f>
+        <v>380.54275092936803</v>
+      </c>
+      <c r="I3" s="11">
+        <f>1023*((E3-$C$11)/($C$13-$C$11))</f>
+        <v>993.44992052753503</v>
+      </c>
+      <c r="J3" s="11">
+        <f t="shared" ref="J3:J4" si="0">I3-H3</f>
+        <v>612.907169598167</v>
+      </c>
+      <c r="K3" s="13"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="9">
+        <v>3.6</v>
+      </c>
+      <c r="B4" s="9">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9">
+        <v>20</v>
+      </c>
+      <c r="D4" s="9">
+        <v>30</v>
+      </c>
+      <c r="E4" s="10">
+        <f>(D4/(((C4^-0.654)*119.78)+(D4)))*A4</f>
+        <v>2.3034901962843417</v>
+      </c>
+      <c r="F4" s="10">
+        <f>(D4/(((B4^-0.654)*119.78)+(D4)))*A4</f>
+        <v>0.72105755107490987</v>
+      </c>
+      <c r="G4" s="10">
+        <f>E4-F4</f>
+        <v>1.5824326452094319</v>
+      </c>
+      <c r="H4" s="11">
+        <f>1023*((F4-$C$11)/($C$13-$C$11))</f>
+        <v>295.05674989985312</v>
+      </c>
+      <c r="I4" s="11">
+        <f>1023*((E4-$C$11)/($C$13-$C$11))</f>
+        <v>942.58818831955273</v>
+      </c>
+      <c r="J4" s="14">
+        <f t="shared" si="0"/>
+        <v>647.53143841969961</v>
+      </c>
+      <c r="K4" s="13"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="9"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="9">
+        <v>5</v>
+      </c>
+      <c r="B6" s="9">
+        <v>1</v>
+      </c>
+      <c r="C6" s="9">
+        <v>20</v>
+      </c>
+      <c r="D6" s="9">
+        <v>40</v>
+      </c>
+      <c r="E6" s="10">
+        <f>(D6/(((C6^-0.654)*119.78)+(D6)))*A6</f>
+        <v>3.5158422096389632</v>
+      </c>
+      <c r="F6" s="10">
+        <f>(D6/(((B6^-0.654)*119.78)+(D6)))*A6</f>
+        <v>1.251721116535236</v>
+      </c>
+      <c r="G6" s="10">
+        <f>E6-F6</f>
+        <v>2.2641210931037272</v>
+      </c>
+      <c r="H6" s="11">
+        <f>1023*((F6-$B$11)/($B$13-$B$11))</f>
+        <v>355.69741728209618</v>
+      </c>
+      <c r="I6" s="11">
+        <f>1023*((E6-$B$11)/($B$13-$B$11))</f>
+        <v>999.08516123907202</v>
+      </c>
+      <c r="J6" s="11">
+        <f>I6-H6</f>
+        <v>643.38774395697578</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="9">
+        <v>3.3</v>
+      </c>
+      <c r="B7" s="9">
+        <v>1</v>
+      </c>
+      <c r="C7" s="9">
+        <v>20</v>
+      </c>
+      <c r="D7" s="9">
+        <v>47</v>
+      </c>
+      <c r="E7" s="10">
+        <f>(D7/(((C7^-0.654)*119.78)+(D7)))*A7</f>
+        <v>2.4277857295394307</v>
+      </c>
+      <c r="F7" s="10">
+        <f>(D7/(((B7^-0.654)*119.78)+(D7)))*A7</f>
+        <v>0.92996762201702843</v>
+      </c>
+      <c r="G7" s="10">
+        <f>E7-F7</f>
+        <v>1.4978181075224022</v>
+      </c>
+      <c r="H7" s="11">
+        <f>1023*((F7-$B$11)/($B$13-$B$11))</f>
+        <v>264.26579925650555</v>
+      </c>
+      <c r="I7" s="11">
+        <f t="shared" ref="I7:I8" si="1">1023*((E7-$B$11)/($B$13-$B$11))</f>
+        <v>689.89577814412155</v>
+      </c>
+      <c r="J7" s="11">
+        <f t="shared" ref="J7:J8" si="2">I7-H7</f>
+        <v>425.62997888761601</v>
+      </c>
+      <c r="K7" s="13"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="9">
+        <v>3.6</v>
+      </c>
+      <c r="B8" s="9">
+        <v>1</v>
+      </c>
+      <c r="C8" s="9">
+        <v>20</v>
+      </c>
+      <c r="D8" s="9">
+        <v>47</v>
+      </c>
+      <c r="E8" s="10">
+        <f>(D8/(((C8^-0.654)*119.78)+(D8)))*A8</f>
+        <v>2.6484935231339244</v>
+      </c>
+      <c r="F8" s="10">
+        <f>(D8/(((B8^-0.654)*119.78)+(D8)))*A8</f>
+        <v>1.0145101331094857</v>
+      </c>
+      <c r="G8" s="10">
+        <f>E8-F8</f>
+        <v>1.6339833900244387</v>
+      </c>
+      <c r="H8" s="11">
+        <f t="shared" ref="H7:H8" si="3">1023*((F8-$B$11)/($B$13-$B$11))</f>
+        <v>288.28996282527885</v>
+      </c>
+      <c r="I8" s="11">
+        <f t="shared" si="1"/>
+        <v>752.61357615722352</v>
+      </c>
+      <c r="J8" s="11">
+        <f t="shared" si="2"/>
+        <v>464.32361333194467</v>
+      </c>
+      <c r="K8" s="13"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="9"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B11" s="9">
+        <v>0</v>
+      </c>
+      <c r="C11" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B13" s="9">
+        <v>3.6</v>
+      </c>
+      <c r="C13" s="9">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B14" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="12"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="L7:P8"/>
-    <mergeCell ref="L10:P11"/>
+    <mergeCell ref="A22:E23"/>
+    <mergeCell ref="K2:K4"/>
+    <mergeCell ref="K6:K8"/>
   </mergeCells>
+  <conditionalFormatting sqref="E2:E5 E10:E1048576">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
+      <formula>$C$13</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E6:E9">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+      <formula>$B$13</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
line pressure vs adc calibration curve
used physical lever amr and piston geometry, values in line with expected line pressures (from professional experience)
</commit_message>
<xml_diff>
--- a/Peripheral Code/Force Sensor/Calibration Data.xlsx
+++ b/Peripheral Code/Force Sensor/Calibration Data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JasonsRazer\Dropbox\Notes\MECH 423 - Mechatronic Product Design\PROJECT\MECH423 Project GIT REPO\CyclingDAQ\Peripheral Code\Force Sensor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B84BF07-16B8-4EA9-BCE9-97BC4D17DA3D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F16ADE6-8D48-4FC2-8C47-A5C3B2E26766}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{55C83500-F648-47C6-B0AB-D5CA633E4192}"/>
+    <workbookView xWindow="-10308" yWindow="4428" windowWidth="17280" windowHeight="8724" activeTab="3" xr2:uid="{55C83500-F648-47C6-B0AB-D5CA633E4192}"/>
   </bookViews>
   <sheets>
     <sheet name="Calibration" sheetId="1" r:id="rId1"/>
     <sheet name="Arduino" sheetId="2" r:id="rId2"/>
     <sheet name="MSP430" sheetId="3" r:id="rId3"/>
+    <sheet name="Testing &amp; Final Calibration" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -69,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
   <si>
     <t>Resistance [kOhm]</t>
   </si>
@@ -148,6 +149,63 @@
   <si>
     <t>Limitation to have 255 max value b/c 8 bits</t>
   </si>
+  <si>
+    <t>Voltage</t>
+  </si>
+  <si>
+    <t>Approx ADC Value</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>lever_long</t>
+  </si>
+  <si>
+    <t>lever_short</t>
+  </si>
+  <si>
+    <t>piston_master</t>
+  </si>
+  <si>
+    <t>piston_caliper</t>
+  </si>
+  <si>
+    <t>diam</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>mm2</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>m2</t>
+  </si>
+  <si>
+    <t>in2</t>
+  </si>
+  <si>
+    <t>RATIO</t>
+  </si>
+  <si>
+    <t>(torque multiplication)</t>
+  </si>
+  <si>
+    <t>Line Pressure (psi)</t>
+  </si>
+  <si>
+    <t>Calibration curve Force [kg]</t>
+  </si>
+  <si>
+    <t>[lbs]</t>
+  </si>
 </sst>
 </file>
 
@@ -191,7 +249,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -224,6 +282,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -232,51 +293,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -791,6 +818,1455 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Force Sensor Calibration Curve (Spec Sheet F</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> vs R)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Calibration!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Resistance [kOhm]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:forward val="0.5"/>
+            <c:backward val="0.2"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.24651071741032371"/>
+                  <c:y val="-0.24459135316418781"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Calibration!$A$3:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>22</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Calibration!$B$3:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6B56-4C1B-85D4-6BF40C95ED43}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="725926624"/>
+        <c:axId val="628120192"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="725926624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="628120192"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="628120192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="725926624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Force Sensor Calibration Curve (F vs ADC)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:forward val="0.5"/>
+            <c:backward val="0.2"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.24651071741032371"/>
+                  <c:y val="-0.24459135316418781"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Testing &amp; Final Calibration'!$A$2:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>22</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Testing &amp; Final Calibration'!$H$2:$H$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>49.500000000000007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>92.399999999999991</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>115.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>125.99999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>145.89473684210526</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>163.05882352941177</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>173.25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>182.36842105263159</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>187.29729729729729</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>198.00000000000003</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>203.82352941176472</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>206.86567164179107</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>210</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5F6F-442A-8EDB-195449575CAF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="725926624"/>
+        <c:axId val="628120192"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="725926624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="628120192"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="628120192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="725926624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Force Sensor Calibration Curve (PSI vs ADC)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:forward val="0.5"/>
+            <c:backward val="0.2"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.24651071741032371"/>
+                  <c:y val="-0.24459135316418781"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="6"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Testing &amp; Final Calibration'!$H$2:$H$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>49.500000000000007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>92.399999999999991</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>115.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>125.99999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>145.89473684210526</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>163.05882352941177</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>173.25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>182.36842105263159</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>187.29729729729729</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>198.00000000000003</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>203.82352941176472</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>206.86567164179107</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>210</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Testing &amp; Final Calibration'!$G$2:$G$16</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23.570430179836265</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>84.230266644611021</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>145.31864019747567</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>183.94434764662685</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>285.57768628085222</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>341.93151994705465</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>419.38398165600501</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>530.85628116480802</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>660.70005156882019</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>746.71935495415573</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>986.80115705883486</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1159.2983878939476</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1265.1784385918927</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1388.0659410305132</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9579-4B3E-A7D0-75987BA1C686}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="725926624"/>
+        <c:axId val="628120192"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="725926624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="628120192"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="628120192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="725926624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -831,7 +2307,1675 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1487,6 +4631,175 @@
         <a:xfrm>
           <a:off x="3695700" y="1914104"/>
           <a:ext cx="6606540" cy="2316579"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>144780</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1165860</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5A6BFEF-913C-48D3-8268-92049B29F5AB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>867591</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>37011</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4795CDC6-B0ED-4C54-A273-6FBECA83EE1E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>21773</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>43544</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>432164</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>43543</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE2CC4E7-3D3D-4342-B00A-724AC5F08722}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>457201</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>108858</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>152401</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>126547</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBC130ED-9542-4E87-B758-6A4CD37E2EBD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9622972" y="5105401"/>
+          <a:ext cx="5715000" cy="3533775"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1818,7 +5131,7 @@
   <dimension ref="A1:T20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="L14" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1828,10 +5141,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="12"/>
+      <c r="B1" s="13"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -2141,36 +5454,36 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="13"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
+      <c r="A7" s="14"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="13"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2185,8 +5498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F15F4A7-B3B1-46FF-8C39-09F79D339A4A}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2273,7 +5586,7 @@
         <f>I2-H2</f>
         <v>1543.8977843308603</v>
       </c>
-      <c r="K2" s="15" t="s">
+      <c r="K2" s="16" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2314,7 +5627,7 @@
         <f t="shared" ref="J3:J4" si="1">I3-H3</f>
         <v>1018.9725376583676</v>
       </c>
-      <c r="K3" s="15"/>
+      <c r="K3" s="16"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
@@ -2353,7 +5666,7 @@
         <f t="shared" si="1"/>
         <v>1111.6064047182192</v>
       </c>
-      <c r="K4" s="15"/>
+      <c r="K4" s="16"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E5" s="8"/>
@@ -2401,7 +5714,7 @@
         <f>I6-H6</f>
         <v>1012.1737161810934</v>
       </c>
-      <c r="K6" s="15" t="s">
+      <c r="K6" s="16" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2442,7 +5755,7 @@
         <f t="shared" ref="J7:J8" si="4">I7-H7</f>
         <v>707.61981781831082</v>
       </c>
-      <c r="K7" s="15"/>
+      <c r="K7" s="16"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
@@ -2481,7 +5794,7 @@
         <f t="shared" si="4"/>
         <v>771.94889216543004</v>
       </c>
-      <c r="K8" s="15"/>
+      <c r="K8" s="16"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E9" s="8"/>
@@ -2536,36 +5849,36 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="14"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
+      <c r="A23" s="15"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="15" t="s">
+      <c r="A25" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="15"/>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
+      <c r="A26" s="16"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2575,7 +5888,7 @@
     <mergeCell ref="A25:E26"/>
   </mergeCells>
   <conditionalFormatting sqref="E10:E24 E27:E1048576 E2:E5">
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
       <formula>$C$13</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2593,4 +5906,652 @@
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B1E972D-BE7C-4075-BAC1-BE110CF59298}">
+  <dimension ref="A1:X20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="I2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="12"/>
+    <col min="2" max="2" width="16.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="16.33203125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="20" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="20" style="12" customWidth="1"/>
+    <col min="8" max="8" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" customWidth="1"/>
+    <col min="11" max="11" width="13.109375" customWidth="1"/>
+    <col min="18" max="18" width="21.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
+      <c r="X1" s="12"/>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A2" s="12">
+        <v>0</v>
+      </c>
+      <c r="B2" s="12">
+        <v>1000</v>
+      </c>
+      <c r="D2" s="17">
+        <v>0</v>
+      </c>
+      <c r="E2" s="17">
+        <v>0</v>
+      </c>
+      <c r="F2" s="17">
+        <f>E2*2.20462</f>
+        <v>0</v>
+      </c>
+      <c r="G2" s="18">
+        <f>(F2*$Q$2)/$R$6</f>
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <f t="shared" ref="H2:H14" si="0">($H$16/$D$16)*D2</f>
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2">
+        <v>60</v>
+      </c>
+      <c r="M2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2">
+        <f>L2/1000</f>
+        <v>0.06</v>
+      </c>
+      <c r="O2" t="s">
+        <v>37</v>
+      </c>
+      <c r="P2" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q2" s="12">
+        <f>N2/N3</f>
+        <v>3.5294117647058818</v>
+      </c>
+      <c r="R2" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="S2" s="12"/>
+      <c r="T2" s="12"/>
+      <c r="U2" s="12"/>
+      <c r="V2" s="12"/>
+      <c r="W2" s="12"/>
+      <c r="X2" s="12"/>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A3" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="B3" s="12">
+        <v>230</v>
+      </c>
+      <c r="D3" s="17">
+        <f t="shared" ref="D3:D16" si="1">(50000/((B3*1000)+50000))*3.6</f>
+        <v>0.6428571428571429</v>
+      </c>
+      <c r="E3" s="17">
+        <f t="shared" ref="E3:E16" si="2">(5989*5989^(173/327))/(250*(2^(173/327))*(5^(19/327))*(B3^(500/327)))</f>
+        <v>0.36876782039370126</v>
+      </c>
+      <c r="F3" s="17">
+        <f t="shared" ref="F3:F16" si="3">E3*2.20462</f>
+        <v>0.81299291219636161</v>
+      </c>
+      <c r="G3" s="18">
+        <f t="shared" ref="G3:G16" si="4">(F3*$Q$2)/$R$6</f>
+        <v>23.570430179836265</v>
+      </c>
+      <c r="H3">
+        <f t="shared" si="0"/>
+        <v>49.500000000000007</v>
+      </c>
+      <c r="K3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3">
+        <v>17</v>
+      </c>
+      <c r="M3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N3">
+        <f>L3/1000</f>
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="O3" t="s">
+        <v>37</v>
+      </c>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="12"/>
+      <c r="S3" s="12"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="4"/>
+      <c r="X3" s="4"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A4" s="12">
+        <v>1</v>
+      </c>
+      <c r="B4" s="12">
+        <v>100</v>
+      </c>
+      <c r="D4" s="17">
+        <f t="shared" si="1"/>
+        <v>1.2</v>
+      </c>
+      <c r="E4" s="17">
+        <f t="shared" si="2"/>
+        <v>1.3178126832952548</v>
+      </c>
+      <c r="F4" s="17">
+        <f t="shared" si="3"/>
+        <v>2.9052761978463844</v>
+      </c>
+      <c r="G4" s="18">
+        <f t="shared" si="4"/>
+        <v>84.230266644611021</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>92.399999999999991</v>
+      </c>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="4"/>
+      <c r="X4" s="4"/>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A5" s="12">
+        <v>2</v>
+      </c>
+      <c r="B5" s="12">
+        <v>70</v>
+      </c>
+      <c r="D5" s="17">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+      <c r="E5" s="17">
+        <f t="shared" si="2"/>
+        <v>2.2735621623929081</v>
+      </c>
+      <c r="F5" s="17">
+        <f t="shared" si="3"/>
+        <v>5.0123406144546525</v>
+      </c>
+      <c r="G5" s="18">
+        <f t="shared" si="4"/>
+        <v>145.31864019747567</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>115.5</v>
+      </c>
+      <c r="L5" t="s">
+        <v>33</v>
+      </c>
+      <c r="N5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A6" s="12">
+        <v>3</v>
+      </c>
+      <c r="B6" s="12">
+        <v>60</v>
+      </c>
+      <c r="D6" s="17">
+        <f t="shared" si="1"/>
+        <v>1.6363636363636362</v>
+      </c>
+      <c r="E6" s="17">
+        <f t="shared" si="2"/>
+        <v>2.877875186742096</v>
+      </c>
+      <c r="F6" s="17">
+        <f t="shared" si="3"/>
+        <v>6.3446211941953594</v>
+      </c>
+      <c r="G6" s="18">
+        <f t="shared" si="4"/>
+        <v>183.94434764662685</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>125.99999999999999</v>
+      </c>
+      <c r="K6" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6">
+        <v>10</v>
+      </c>
+      <c r="M6" t="s">
+        <v>28</v>
+      </c>
+      <c r="N6">
+        <f>PI()*(L6/2)^2</f>
+        <v>78.539816339744831</v>
+      </c>
+      <c r="O6" t="s">
+        <v>36</v>
+      </c>
+      <c r="P6" s="6">
+        <f>N6/1000000</f>
+        <v>7.8539816339744827E-5</v>
+      </c>
+      <c r="Q6" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="R6" s="6">
+        <f>N6*0.00155</f>
+        <v>0.12173671532660449</v>
+      </c>
+      <c r="S6" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="T6" s="6"/>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A7" s="12">
+        <v>4</v>
+      </c>
+      <c r="B7" s="12">
+        <v>45</v>
+      </c>
+      <c r="D7" s="17">
+        <f t="shared" si="1"/>
+        <v>1.8947368421052631</v>
+      </c>
+      <c r="E7" s="17">
+        <f t="shared" si="2"/>
+        <v>4.4679651631032566</v>
+      </c>
+      <c r="F7" s="17">
+        <f t="shared" si="3"/>
+        <v>9.8501653578807016</v>
+      </c>
+      <c r="G7" s="18">
+        <f t="shared" si="4"/>
+        <v>285.57768628085222</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>145.89473684210526</v>
+      </c>
+      <c r="K7" t="s">
+        <v>32</v>
+      </c>
+      <c r="L7">
+        <v>22</v>
+      </c>
+      <c r="M7" t="s">
+        <v>28</v>
+      </c>
+      <c r="N7">
+        <f>PI()*(L7/2)^2</f>
+        <v>380.13271108436498</v>
+      </c>
+      <c r="O7" t="s">
+        <v>36</v>
+      </c>
+      <c r="P7" s="6">
+        <f>N7/1000000</f>
+        <v>3.8013271108436499E-4</v>
+      </c>
+      <c r="Q7" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="R7" s="6">
+        <f>N7*0.00155</f>
+        <v>0.58920570218076573</v>
+      </c>
+      <c r="S7" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="T7" s="6"/>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A8" s="12">
+        <v>5</v>
+      </c>
+      <c r="B8" s="12">
+        <v>40</v>
+      </c>
+      <c r="D8" s="17">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E8" s="17">
+        <f t="shared" si="2"/>
+        <v>5.3496410703038189</v>
+      </c>
+      <c r="F8" s="17">
+        <f t="shared" si="3"/>
+        <v>11.793925696413204</v>
+      </c>
+      <c r="G8" s="18">
+        <f t="shared" si="4"/>
+        <v>341.93151994705465</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>154</v>
+      </c>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A9" s="12">
+        <v>7</v>
+      </c>
+      <c r="B9" s="12">
+        <v>35</v>
+      </c>
+      <c r="D9" s="17">
+        <f t="shared" si="1"/>
+        <v>2.1176470588235294</v>
+      </c>
+      <c r="E9" s="17">
+        <f t="shared" si="2"/>
+        <v>6.5614125683467384</v>
+      </c>
+      <c r="F9" s="17">
+        <f t="shared" si="3"/>
+        <v>14.465421376428585</v>
+      </c>
+      <c r="G9" s="18">
+        <f t="shared" si="4"/>
+        <v>419.38398165600501</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>163.05882352941177</v>
+      </c>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A10" s="12">
+        <v>9</v>
+      </c>
+      <c r="B10" s="12">
+        <v>30</v>
+      </c>
+      <c r="D10" s="17">
+        <f t="shared" si="1"/>
+        <v>2.25</v>
+      </c>
+      <c r="E10" s="17">
+        <f t="shared" si="2"/>
+        <v>8.3054366107802604</v>
+      </c>
+      <c r="F10" s="17">
+        <f t="shared" si="3"/>
+        <v>18.310331660858377</v>
+      </c>
+      <c r="G10" s="18">
+        <f t="shared" si="4"/>
+        <v>530.85628116480802</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>173.25</v>
+      </c>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A11" s="12">
+        <v>11</v>
+      </c>
+      <c r="B11" s="12">
+        <v>26</v>
+      </c>
+      <c r="D11" s="17">
+        <f t="shared" si="1"/>
+        <v>2.3684210526315792</v>
+      </c>
+      <c r="E11" s="17">
+        <f t="shared" si="2"/>
+        <v>10.336888893927364</v>
+      </c>
+      <c r="F11" s="17">
+        <f t="shared" si="3"/>
+        <v>22.788911993330142</v>
+      </c>
+      <c r="G11" s="18">
+        <f t="shared" si="4"/>
+        <v>660.70005156882019</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>182.36842105263159</v>
+      </c>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6"/>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A12" s="12">
+        <v>13</v>
+      </c>
+      <c r="B12" s="12">
+        <v>24</v>
+      </c>
+      <c r="D12" s="17">
+        <f t="shared" si="1"/>
+        <v>2.4324324324324325</v>
+      </c>
+      <c r="E12" s="17">
+        <f t="shared" si="2"/>
+        <v>11.682691697659436</v>
+      </c>
+      <c r="F12" s="17">
+        <f t="shared" si="3"/>
+        <v>25.755895770493943</v>
+      </c>
+      <c r="G12" s="18">
+        <f t="shared" si="4"/>
+        <v>746.71935495415573</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>187.29729729729729</v>
+      </c>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="6"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A13" s="12">
+        <v>15</v>
+      </c>
+      <c r="B13" s="12">
+        <v>20</v>
+      </c>
+      <c r="D13" s="17">
+        <f t="shared" si="1"/>
+        <v>2.5714285714285716</v>
+      </c>
+      <c r="E13" s="17">
+        <f t="shared" si="2"/>
+        <v>15.43885746140832</v>
+      </c>
+      <c r="F13" s="17">
+        <f t="shared" si="3"/>
+        <v>34.036813936570006</v>
+      </c>
+      <c r="G13" s="18">
+        <f t="shared" si="4"/>
+        <v>986.80115705883486</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>198.00000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A14" s="12">
+        <v>17</v>
+      </c>
+      <c r="B14" s="12">
+        <v>18</v>
+      </c>
+      <c r="D14" s="17">
+        <f t="shared" si="1"/>
+        <v>2.6470588235294121</v>
+      </c>
+      <c r="E14" s="17">
+        <f t="shared" si="2"/>
+        <v>18.137638406587303</v>
+      </c>
+      <c r="F14" s="17">
+        <f t="shared" si="3"/>
+        <v>39.986600383930494</v>
+      </c>
+      <c r="G14" s="18">
+        <f t="shared" si="4"/>
+        <v>1159.2983878939476</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>203.82352941176472</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A15" s="12">
+        <v>20</v>
+      </c>
+      <c r="B15" s="12">
+        <v>17</v>
+      </c>
+      <c r="D15" s="17">
+        <f t="shared" si="1"/>
+        <v>2.6865671641791047</v>
+      </c>
+      <c r="E15" s="17">
+        <f t="shared" si="2"/>
+        <v>19.794169713871526</v>
+      </c>
+      <c r="F15" s="17">
+        <f t="shared" si="3"/>
+        <v>43.63862243459544</v>
+      </c>
+      <c r="G15" s="18">
+        <f t="shared" si="4"/>
+        <v>1265.1784385918927</v>
+      </c>
+      <c r="H15">
+        <f>($H$16/$D$16)*D15</f>
+        <v>206.86567164179107</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A16" s="12">
+        <v>22</v>
+      </c>
+      <c r="B16" s="12">
+        <v>16</v>
+      </c>
+      <c r="D16" s="17">
+        <f t="shared" si="1"/>
+        <v>2.7272727272727275</v>
+      </c>
+      <c r="E16" s="17">
+        <f t="shared" si="2"/>
+        <v>21.716788693761121</v>
+      </c>
+      <c r="F16" s="17">
+        <f t="shared" si="3"/>
+        <v>47.87726669003964</v>
+      </c>
+      <c r="G16" s="18">
+        <f t="shared" si="4"/>
+        <v>1388.0659410305132</v>
+      </c>
+      <c r="H16">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20"/>
+      <c r="C20"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>